<commit_message>
added last two graphs for part 3
</commit_message>
<xml_diff>
--- a/testoutput3.xlsx
+++ b/testoutput3.xlsx
@@ -1191,11 +1191,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="172591360"/>
-        <c:axId val="172597248"/>
+        <c:axId val="182880896"/>
+        <c:axId val="182882688"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="172591360"/>
+        <c:axId val="182880896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1205,12 +1205,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172597248"/>
+        <c:crossAx val="182882688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="172597248"/>
+        <c:axId val="182882688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,7 +1221,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="172591360"/>
+        <c:crossAx val="182880896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1858,11 +1858,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="174392064"/>
-        <c:axId val="174393600"/>
+        <c:axId val="184353920"/>
+        <c:axId val="184355456"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="174392064"/>
+        <c:axId val="184353920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1872,12 +1872,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174393600"/>
+        <c:crossAx val="184355456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="174393600"/>
+        <c:axId val="184355456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1888,7 +1888,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174392064"/>
+        <c:crossAx val="184353920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2525,11 +2525,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="64546688"/>
-        <c:axId val="64545152"/>
+        <c:axId val="184368512"/>
+        <c:axId val="184398976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="64546688"/>
+        <c:axId val="184368512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2539,12 +2539,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64545152"/>
+        <c:crossAx val="184398976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="64545152"/>
+        <c:axId val="184398976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2555,7 +2555,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64546688"/>
+        <c:crossAx val="184368512"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3192,11 +3192,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="178266496"/>
-        <c:axId val="178264704"/>
+        <c:axId val="185075584"/>
+        <c:axId val="185077120"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178266496"/>
+        <c:axId val="185075584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3206,12 +3206,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178264704"/>
+        <c:crossAx val="185077120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="178264704"/>
+        <c:axId val="185077120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3222,7 +3222,1341 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178266496"/>
+        <c:crossAx val="185075584"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>testoutput3!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Number of probes to determine entry isn't present</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>testoutput3!$A$2:$A$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>testoutput3!$F$2:$F$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>0.1069</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.1027</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.13769999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.18659999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.1865</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.1976</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.2094</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25090000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.25269999999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.25629999999999997</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.30559999999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.2989</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.3246</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.35599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.36349999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.36570000000000003</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.44109999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.46010000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.46779999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.49919999999999998</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.50609999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.56069999999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.57969999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.62050000000000005</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.69510000000000005</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.71199999999999997</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.74829999999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.7863</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.76180000000000003</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.87629999999999997</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.92669999999999997</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.97009999999999996</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>1.0104</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>1.0288999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>1.1456999999999999</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.2188000000000001</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>1.2806999999999999</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1.2648999999999999</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.4342999999999999</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.5088999999999999</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1.5984</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1.5447</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1.6616</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1.7947</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.9378</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>2.0085999999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.2538</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>2.4007000000000001</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.4504999999999999</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>2.5903</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>2.7957999999999998</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>2.4557000000000002</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.1086999999999998</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3.391</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.3662999999999998</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3.6334</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4.0608000000000004</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.1363000000000003</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.6826999999999996</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.0910000000000002</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.367</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5.8501000000000003</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.2843999999999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>6.6447000000000003</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7.4326999999999996</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.8617999999999997</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>8.7317</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>9.4216999999999995</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>10.6683</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>11.6243</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>13.2349</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>14.561199999999999</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>16.575299999999999</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>18.7197</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>20.1541</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>24.1295</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>28.1937</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>33.955599999999997</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>35.356900000000003</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>48.725499999999997</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>57.7241</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>76.471800000000002</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>99.687799999999996</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>136.5866</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>131.50659999999999</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>291.77960000000002</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>571.46019999999999</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1092.4884</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>3940.8188</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>249949.2242</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="185096064"/>
+        <c:axId val="185097600"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="185096064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="185097600"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="185097600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="185096064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>testoutput3!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average time to determine entry isn't present</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>testoutput3!$A$2:$A$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.13</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.14000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.17</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.18</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.19</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.21</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.22</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.23</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.26</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.28000000000000003</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.32</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.34</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.35</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.36</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.43</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.45</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.47</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.48</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.49</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.56000000000000005</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.56999999999999995</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.59</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.62</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.64</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.65</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0.71</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>0.72</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0.76</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0.77</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0.78</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>0.81</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>0.82</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>0.83</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>0.87</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>0.9</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>0.92</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>0.95</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>0.97</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>0.98</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>testoutput3!$G$2:$G$92</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="91"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.6000000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>1.5E-3</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>3.2000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>3.2000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>4.7000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>4.7000000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>6.1999999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>1.5599999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>3.1199999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>0.12479999999999999</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>8.7773000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="185109120"/>
+        <c:axId val="185221504"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="185109120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="185221504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="185221504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="185109120"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3361,6 +4695,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>314324</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="10" name="Chart 9"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3658,11 +5052,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>